<commit_message>
update Analisi Gerarchica, prima divisione in cluster e misure di non omogeneità
</commit_message>
<xml_diff>
--- a/DataSetForR.xlsx
+++ b/DataSetForR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carmi\Desktop\Unisa Magistrale\SAD\SAD_Alcol_Consume_Italy_2019\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01089F73-471F-4620-83C0-750A6D5A3698}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00B3AFBF-D6AD-432C-A2C6-E83492A74D75}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{3EA12E6F-9D00-4C5C-A91F-481F1E6401BC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{3EA12E6F-9D00-4C5C-A91F-481F1E6401BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Foglio1" sheetId="1" r:id="rId1"/>
@@ -35,24 +35,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="27">
   <si>
     <t xml:space="preserve"> Piemonte</t>
   </si>
   <si>
-    <t xml:space="preserve"> Valle d'Aosta/Vallée d'Aoste</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Liguria</t>
   </si>
   <si>
     <t xml:space="preserve"> Lombardia</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Trentino-Alto Adige</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bolzano/Bozen</t>
   </si>
   <si>
     <t xml:space="preserve"> Trento</t>
@@ -197,7 +188,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -234,8 +225,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -258,12 +261,49 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -312,6 +352,29 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -320,6 +383,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFF66"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -630,7 +698,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9435E24-E0EF-4BCD-AF63-DE7ACF81D5AA}">
   <dimension ref="A1:F34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B1" sqref="B1:F22"/>
     </sheetView>
   </sheetViews>
@@ -646,22 +714,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="B1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -686,7 +754,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B3" s="5">
         <v>54</v>
@@ -706,7 +774,7 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="5">
         <v>715</v>
@@ -726,7 +794,7 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="16" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="5">
         <v>4746</v>
@@ -746,7 +814,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="16" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B6" s="5">
         <v>225</v>
@@ -766,7 +834,7 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="16" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="B7" s="5">
         <v>244</v>
@@ -786,7 +854,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8" s="5">
         <v>2390</v>
@@ -806,7 +874,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B9" s="5">
         <v>578</v>
@@ -826,7 +894,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10" s="5">
         <v>2091</v>
@@ -846,7 +914,7 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="16" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B11" s="5">
         <v>1769</v>
@@ -866,7 +934,7 @@
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="16" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B12" s="5">
         <v>418</v>
@@ -886,7 +954,7 @@
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="16" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B13" s="5">
         <v>708</v>
@@ -906,7 +974,7 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="16" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B14" s="5">
         <v>2847</v>
@@ -926,7 +994,7 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="16" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B15" s="5">
         <v>596</v>
@@ -946,7 +1014,7 @@
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="16" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B16" s="5">
         <v>138</v>
@@ -966,7 +1034,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="16" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B17" s="5">
         <v>2565</v>
@@ -986,7 +1054,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="16" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B18" s="5">
         <v>1869</v>
@@ -1006,7 +1074,7 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="16" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B19" s="5">
         <v>264</v>
@@ -1026,7 +1094,7 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="16" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B20" s="5">
         <v>903</v>
@@ -1046,7 +1114,7 @@
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" s="16" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B21" s="5">
         <v>2330</v>
@@ -1066,7 +1134,7 @@
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" s="16" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B22" s="5">
         <v>683</v>
@@ -1153,8 +1221,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{280E646D-18DD-4657-A2F3-93B8C5C386BB}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1168,19 +1236,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>23</v>
-      </c>
-      <c r="C1" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D1" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
@@ -1547,130 +1615,161 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C0E1902-A7BD-440A-BCB0-2F90BD4FAA5A}">
-  <dimension ref="A1:A23"/>
+  <dimension ref="A1:B22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A23"/>
+      <selection sqref="A1:B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
+    <col min="2" max="2" width="17.5546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" s="17"/>
+      <c r="B1" s="17" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="21">
+        <v>1</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="25">
+        <v>2</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="26"/>
+      <c r="B4" s="19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="26"/>
+      <c r="B5" s="19" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="26"/>
+      <c r="B6" s="19" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="26"/>
+      <c r="B7" s="19" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="26"/>
+      <c r="B8" s="19" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="26"/>
+      <c r="B9" s="19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="26"/>
+      <c r="B10" s="19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="26"/>
+      <c r="B11" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="26"/>
+      <c r="B12" s="19" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="26"/>
+      <c r="B13" s="19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="27"/>
+      <c r="B14" s="19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="22">
+        <v>3</v>
+      </c>
+      <c r="B15" s="20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="23"/>
+      <c r="B16" s="20" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="23"/>
+      <c r="B17" s="20" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="23"/>
+      <c r="B18" s="20" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="23"/>
+      <c r="B19" s="20" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="23"/>
+      <c r="B20" s="20" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="23"/>
+      <c r="B21" s="20" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="24"/>
+      <c r="B22" s="20" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>21</v>
-      </c>
-    </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A3:A14"/>
+    <mergeCell ref="A15:A22"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>